<commit_message>
minor changes to docmentation
</commit_message>
<xml_diff>
--- a/Output/QSAR_predictions_database_content_descriptions.xlsx
+++ b/Output/QSAR_predictions_database_content_descriptions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\QSAR_predictions_database\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{46504584-CD5F-4885-85E3-0D0E7C4C8BE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58ED809A-8B9A-42FB-BB75-235B5F33280A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31845" yWindow="1665" windowWidth="25680" windowHeight="17400" xr2:uid="{2D05DBB1-4549-420F-9A87-95D458EF22FE}"/>
+    <workbookView xWindow="15" yWindow="0" windowWidth="25170" windowHeight="15150" activeTab="2" xr2:uid="{2D05DBB1-4549-420F-9A87-95D458EF22FE}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="4" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3783" uniqueCount="1025">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3782" uniqueCount="1024">
   <si>
     <t>META_QSARn</t>
   </si>
@@ -3112,9 +3112,6 @@
   </si>
   <si>
     <t>Molecular weights collected to translate from molar units to mg per liter</t>
-  </si>
-  <si>
-    <t>fdf</t>
   </si>
 </sst>
 </file>
@@ -3763,9 +3760,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D36B2048-821C-47B0-B3EF-7894A4F59796}">
-  <dimension ref="B3:G15"/>
+  <dimension ref="B3:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -3822,11 +3819,6 @@
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>680</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>1024</v>
       </c>
     </row>
   </sheetData>
@@ -14596,8 +14588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF8AE417-D626-486A-87C0-78912EF60B00}">
   <dimension ref="B2:F331"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView tabSelected="1" topLeftCell="A293" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>